<commit_message>
Serial python working with Arduino, Accel not working anymore
</commit_message>
<xml_diff>
--- a/Software/Serial_Communication_Code.xlsx
+++ b/Software/Serial_Communication_Code.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BartendUS-GROS4\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F38D507-3A5D-476A-BF5A-6FDC6E8576B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADA8590-F8FC-46FA-8586-9DD83539564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{2575488B-D410-4C95-B48D-D1D1AAD5D153}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{2575488B-D410-4C95-B48D-D1D1AAD5D153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,14 +23,41 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Move motor</t>
+  </si>
+  <si>
+    <t>Change speed</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,14 +407,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9769F1A-8714-4ADB-8B62-CD7F3A68593F}">
-  <dimension ref="A1"/>
+  <dimension ref="C4:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="4" width="1.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>